<commit_message>
:100: Dummy Data Plot Complete
</commit_message>
<xml_diff>
--- a/dummydata.xlsx
+++ b/dummydata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Araf\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Araf\PycharmProjects\BasicPython\NesternShip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{892DAE48-F265-4A3A-8910-AF08E0E21C04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23336FE7-4C07-42E5-8957-1B285F84276C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="960" windowWidth="15375" windowHeight="7875" xr2:uid="{445C3BC8-79E2-41DC-84A6-25A98777F70A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{445C3BC8-79E2-41DC-84A6-25A98777F70A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">Name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID </t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Araf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subangkar </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Employee Name </t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Mr. A</t>
+  </si>
+  <si>
+    <t>Mr. B</t>
+  </si>
+  <si>
+    <t>Mr. C</t>
+  </si>
+  <si>
+    <t>Mr. D</t>
+  </si>
+  <si>
+    <t>Mr. E</t>
+  </si>
+  <si>
+    <t>Mr. F</t>
   </si>
 </sst>
 </file>
@@ -75,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,15 +407,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7F54C5-79E1-4C64-9E49-C178448E28D9}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,27 +428,176 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44100</v>
+      </c>
+      <c r="D2">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44100</v>
+      </c>
+      <c r="D3">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>1505009</v>
-      </c>
-      <c r="C2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4" s="1">
+        <v>44100</v>
+      </c>
+      <c r="D4">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>1505015</v>
-      </c>
-      <c r="C3">
-        <v>23</v>
+      <c r="C5" s="1">
+        <v>44100</v>
+      </c>
+      <c r="D5">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44100</v>
+      </c>
+      <c r="D6">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44100</v>
+      </c>
+      <c r="D7">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44101</v>
+      </c>
+      <c r="D8">
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44101</v>
+      </c>
+      <c r="D9">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44101</v>
+      </c>
+      <c r="D10">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44101</v>
+      </c>
+      <c r="D11">
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44101</v>
+      </c>
+      <c r="D12">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44101</v>
+      </c>
+      <c r="D13">
+        <v>36.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>